<commit_message>
inicial improvements to excel upload
</commit_message>
<xml_diff>
--- a/HaverDevProject/wwwroot/templates/item-upload-template.xlsx
+++ b/HaverDevProject/wwwroot/templates/item-upload-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B574CFA8-6ECD-4E8D-87CA-2A38BBBF07C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662E9125-60B8-4BEF-91C7-AE8081260CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Tension Bolt, ~ KS ~ 5.5 ST</t>
-  </si>
-  <si>
-    <t>profile, C R 49.25 ~ 1.75 C/H</t>
-  </si>
-  <si>
-    <t>Retarding Curtain</t>
-  </si>
-  <si>
-    <t>Side Plate</t>
-  </si>
-  <si>
-    <t>wear protection, PL SW 0.75 4 ~ 48 ~ ~</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>SAP No.</t>
   </si>
@@ -63,6 +48,9 @@
   </si>
   <si>
     <t>Defect Types (Reasons to Reject)</t>
+  </si>
+  <si>
+    <t>Supplier Code</t>
   </si>
 </sst>
 </file>
@@ -457,71 +445,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D3389F-2737-4AAC-865C-901D336B7C41}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
     <col min="2" max="2" width="32.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>200000046</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>200000114</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>200000503</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>200000541</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>200000572</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>